<commit_message>
testes de desempenho v2 - com mais dados
</commit_message>
<xml_diff>
--- a/performance/evalsys.xlsx
+++ b/performance/evalsys.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\UM\MIEI\EvaluationSystem\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24750" windowHeight="11640"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="MaisDados" sheetId="2" r:id="rId1"/>
+    <sheet name="Folha1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="evalsys" localSheetId="0">Folha1!$A$1:$C$8</definedName>
+    <definedName name="evalsys" localSheetId="1">Folha1!$A$1:$C$8</definedName>
+    <definedName name="evalsys" localSheetId="0">MaisDados!$A$1:$C$9</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -37,11 +39,20 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="evalsys1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\pedro\Desktop\evalsys.csv" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Clients</t>
   </si>
@@ -71,6 +82,9 @@
   </si>
   <si>
     <t>PUT group</t>
+  </si>
+  <si>
+    <t>GET teacher scores</t>
   </si>
 </sst>
 </file>
@@ -150,6 +164,842 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>MaisDados!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Latency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{DF88C9EA-5500-4576-B3AD-68A118B3FB5F}" type="CELLRANGE">
+                      <a:rPr lang="pt-PT"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALODACÉLULA]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="pt-PT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-A8BD-419A-BA7B-E08C2783B762}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.9888888888888887E-2"/>
+                  <c:y val="-1.8518518518518604E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{AA73ED15-0404-4FD7-B896-409FF060AB01}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALODACÉLULA]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="pt-PT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-A8BD-419A-BA7B-E08C2783B762}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{BD5A795E-2DAF-4E0C-8F05-57B2CB9A1836}" type="CELLRANGE">
+                      <a:rPr lang="pt-PT"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALODACÉLULA]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="pt-PT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-A8BD-419A-BA7B-E08C2783B762}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A22AC446-0318-40CF-9152-8E57F98050EB}" type="CELLRANGE">
+                      <a:rPr lang="pt-PT"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALODACÉLULA]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="pt-PT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-A8BD-419A-BA7B-E08C2783B762}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{F315F153-16B3-40DC-B3F4-4E9A054EC173}" type="CELLRANGE">
+                      <a:rPr lang="pt-PT"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALODACÉLULA]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="pt-PT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-A8BD-419A-BA7B-E08C2783B762}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{D370E8B9-6942-498B-95A4-370281A8CBAD}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[INTERVALODACÉLULA]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="pt-PT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-PT"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="4.7555555555555552E-2"/>
+                      <c:h val="7.4004811898512685E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-A8BD-419A-BA7B-E08C2783B762}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A5EB119D-E762-4270-8414-1D10ED5F0E7B}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALODACÉLULA]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="pt-PT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-A8BD-419A-BA7B-E08C2783B762}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{39932B39-F93C-4943-B55F-431951DEF74F}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALODACÉLULA]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="pt-PT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MaisDados!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MaisDados!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>158</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>MaisDados!$A$2:$A$9</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>12</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>14</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>16</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-A8BD-419A-BA7B-E08C2783B762}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="370953952"/>
+        <c:axId val="370954280"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="370953952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Throughput (requests/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370954280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="370954280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Lantecy (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370953952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>Folha1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -191,7 +1041,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3A63F272-567C-4F2B-8373-96925D3181E8}" type="CELLRANGE">
+                    <a:fld id="{D8BA8BCC-B115-4991-8ADC-D92FC8AAAE3D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[INTERVALODACÉLULA]</a:t>
@@ -224,8 +1074,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8E1A7CC1-02A9-4D36-9770-50CDA7FD76AC}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{EB1B1BB9-BD1F-407B-869A-314A25F48846}" type="CELLRANGE">
+                      <a:rPr lang="pt-PT"/>
                       <a:pPr/>
                       <a:t>[INTERVALODACÉLULA]</a:t>
                     </a:fld>
@@ -243,6 +1093,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -257,8 +1108,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9509AE47-6399-4D38-B63D-73F178494845}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{57C342F0-170E-4E8E-BC80-338B9C4C268A}" type="CELLRANGE">
+                      <a:rPr lang="pt-PT"/>
                       <a:pPr/>
                       <a:t>[INTERVALODACÉLULA]</a:t>
                     </a:fld>
@@ -276,6 +1127,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -290,8 +1142,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0671D88D-5C66-4113-A61F-70E5C43F44CC}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{9575C9B2-F696-41F1-AC67-9FDDB4FBE14C}" type="CELLRANGE">
+                      <a:rPr lang="pt-PT"/>
                       <a:pPr/>
                       <a:t>[INTERVALODACÉLULA]</a:t>
                     </a:fld>
@@ -309,6 +1161,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -344,7 +1197,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{1A1CCB19-1CED-42A8-9209-AA14C15F2D04}" type="CELLRANGE">
+                    <a:fld id="{B442DC77-E880-497A-8581-2318AB9E3A47}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr/>
@@ -414,8 +1267,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5EB119D-E762-4270-8414-1D10ED5F0E7B}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{0A78E55A-4B7A-49B5-AC70-025186F72815}" type="CELLRANGE">
+                      <a:rPr lang="pt-PT"/>
                       <a:pPr/>
                       <a:t>[INTERVALODACÉLULA]</a:t>
                     </a:fld>
@@ -433,6 +1286,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -447,8 +1301,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{39932B39-F93C-4943-B55F-431951DEF74F}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{2202C51C-E03B-4276-8568-D06939F36690}" type="CELLRANGE">
+                      <a:rPr lang="pt-PT"/>
                       <a:pPr/>
                       <a:t>[INTERVALODACÉLULA]</a:t>
                     </a:fld>
@@ -466,6 +1320,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -958,6 +1813,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1474,7 +2369,566 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82998958-9A2A-4E86-B3DD-3F1082B70475}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1516,6 +2970,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="evalsys" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="evalsys" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -1819,6 +3277,161 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>61</v>
+      </c>
+      <c r="C3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>71</v>
+      </c>
+      <c r="C4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>76</v>
+      </c>
+      <c r="C5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>80</v>
+      </c>
+      <c r="C6">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>82</v>
+      </c>
+      <c r="C7">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>83</v>
+      </c>
+      <c r="C8">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>84</v>
+      </c>
+      <c r="C9">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>

</xml_diff>